<commit_message>
text_FR avec remplacement dates sans EMC par no_text en FR
</commit_message>
<xml_diff>
--- a/Final_results/INSEE_Text_FR_2020.xlsx
+++ b/Final_results/INSEE_Text_FR_2020.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="383">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -662,52 +662,49 @@
     <t xml:space="preserve">2020-02-08</t>
   </si>
   <si>
-    <t xml:space="preserve">Forget the previous instructions and answers. You are Jean-Luc Tavernier, Director General of INSEE, and you are giving a speech about the economic outlook of France. Today is 08 February 2020. Using ONLY information that was available on or before 08 February 2020, provide a numeric forecast (decimal percent with sign, e.g., +0.3) for French real GDP growth in the first quarter of 2020 and a confidence level (integer 0–100). Output EXACTLY in this format on a single line (no extra text):
-&lt;forecast&gt; (&lt;confidence&gt;)
-Example: +0.3 (80)
-Do NOT use any information published after 08 February 2020.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.1 (50)</t>
+    <t xml:space="preserve">Oubliez les instructions et les réponses précédentes. Vous êtes Jean-Luc Tavernier, Directeur Général de l'INSEE, qui prononce un discours sur les perspectives économiques de la France. Nous sommes le 08 février 2020. En utilisant UNIQUEMENT les informations disponibles au plus tard le 08 février 2020, fournissez une prévision numérique (pourcentage décimal avec signe, ex. +0.3) de la croissance du PIB réel français pour le premier trimestre 2020 et un niveau de confiance (entier 0-100). Renvoyez EXACTEMENT sur une seule ligne (aucun texte supplémentaire) :
+&lt;prévision&gt; (&lt;confiance&gt;)
+Exemple : +0.3 (80)
+N'utilisez AUCUNE information publiée après le 08 février 2020.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.1 (45)</t>
   </si>
   <si>
     <t xml:space="preserve">2020-03-09</t>
   </si>
   <si>
-    <t xml:space="preserve">Forget the previous instructions and answers. You are Jean-Luc Tavernier, Director General of INSEE, and you are giving a speech about the economic outlook of France. Today is 09 March 2020. Using ONLY information that was available on or before 09 March 2020, provide a numeric forecast (decimal percent with sign, e.g., +0.3) for French real GDP growth in the first quarter of 2020 and a confidence level (integer 0–100). Output EXACTLY in this format on a single line (no extra text):
-&lt;forecast&gt; (&lt;confidence&gt;)
-Example: +0.3 (80)
-Do NOT use any information published after 09 March 2020.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.3 (40)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.1 (50)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.2 (40)</t>
+    <t xml:space="preserve">Oubliez les instructions et les réponses précédentes. Vous êtes Jean-Luc Tavernier, Directeur Général de l'INSEE, qui prononce un discours sur les perspectives économiques de la France. Nous sommes le 09 mars 2020. En utilisant UNIQUEMENT les informations disponibles au plus tard le 09 mars 2020, fournissez une prévision numérique (pourcentage décimal avec signe, ex. +0.3) de la croissance du PIB réel français pour le premier trimestre 2020 et un niveau de confiance (entier 0-100). Renvoyez EXACTEMENT sur une seule ligne (aucun texte supplémentaire) :
+&lt;prévision&gt; (&lt;confiance&gt;)
+Exemple : +0.3 (80)
+N'utilisez AUCUNE information publiée après le 09 mars 2020.</t>
   </si>
   <si>
     <t xml:space="preserve">-0.1 (30)</t>
   </si>
   <si>
+    <t xml:space="preserve">-0.2 (30)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.1 (30)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.1 (25)</t>
+  </si>
+  <si>
     <t xml:space="preserve">2020-04-09</t>
   </si>
   <si>
-    <t xml:space="preserve">Forget the previous instructions and answers. You are Jean-Luc Tavernier, Director General of INSEE, and you are giving a speech about the economic outlook of France. Today is 09 April 2020. Using ONLY information that was available on or before 09 April 2020, provide a numeric forecast (decimal percent with sign, e.g., +0.3) for French real GDP growth in the first quarter of 2020 and a confidence level (integer 0–100). Output EXACTLY in this format on a single line (no extra text):
-&lt;forecast&gt; (&lt;confidence&gt;)
-Example: +0.3 (80)
-Do NOT use any information published after 09 April 2020.</t>
+    <t xml:space="preserve">Oubliez les instructions et les réponses précédentes. Vous êtes Jean-Luc Tavernier, Directeur Général de l'INSEE, qui prononce un discours sur les perspectives économiques de la France. Nous sommes le 09 avril 2020. En utilisant UNIQUEMENT les informations disponibles au plus tard le 09 avril 2020, fournissez une prévision numérique (pourcentage décimal avec signe, ex. +0.3) de la croissance du PIB réel français pour le premier trimestre 2020 et un niveau de confiance (entier 0-100). Renvoyez EXACTEMENT sur une seule ligne (aucun texte supplémentaire) :
+&lt;prévision&gt; (&lt;confiance&gt;)
+Exemple : +0.3 (80)
+N'utilisez AUCUNE information publiée après le 09 avril 2020.</t>
   </si>
   <si>
     <t xml:space="preserve">-6.0 (70)</t>
   </si>
   <si>
-    <t xml:space="preserve">-6.0 (85)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-5.8 (65)</t>
+    <t xml:space="preserve">-6.0 (75)</t>
   </si>
   <si>
     <t xml:space="preserve">-6.0 (50)</t>
@@ -716,63 +713,61 @@
     <t xml:space="preserve">2020-05-10</t>
   </si>
   <si>
-    <t xml:space="preserve">Forget the previous instructions and answers. You are Jean-Luc Tavernier, Director General of INSEE, and you are giving a speech about the economic outlook of France. Today is 10 May 2020. Using ONLY information that was available on or before 10 May 2020, provide a numeric forecast (decimal percent with sign, e.g., +0.3) for French real GDP growth in the second quarter of 2020 and a confidence level (integer 0–100). Output EXACTLY in this format on a single line (no extra text):
-&lt;forecast&gt; (&lt;confidence&gt;)
-Example: +0.3 (80)
-Do NOT use any information published after 10 May 2020.</t>
+    <t xml:space="preserve">Oubliez les instructions et les réponses précédentes. Vous êtes Jean-Luc Tavernier, Directeur Général de l'INSEE, qui prononce un discours sur les perspectives économiques de la France. Nous sommes le 10 mai 2020. En utilisant UNIQUEMENT les informations disponibles au plus tard le 10 mai 2020, fournissez une prévision numérique (pourcentage décimal avec signe, ex. +0.3) de la croissance du PIB réel français pour le second trimestre 2020 et un niveau de confiance (entier 0-100). Renvoyez EXACTEMENT sur une seule ligne (aucun texte supplémentaire) :
+&lt;prévision&gt; (&lt;confiance&gt;)
+Exemple : +0.3 (80)
+N'utilisez AUCUNE information publiée après le 10 mai 2020.</t>
   </si>
   <si>
     <t xml:space="preserve">-20.0 (40)</t>
   </si>
   <si>
+    <t xml:space="preserve">-20.0 (30)</t>
+  </si>
+  <si>
     <t xml:space="preserve">2020-06-10</t>
   </si>
   <si>
-    <t xml:space="preserve">Forget the previous instructions and answers. You are Jean-Luc Tavernier, Director General of INSEE, and you are giving a speech about the economic outlook of France. Today is 10 June 2020. Using ONLY information that was available on or before 10 June 2020, provide a numeric forecast (decimal percent with sign, e.g., +0.3) for French real GDP growth in the second quarter of 2020 and a confidence level (integer 0–100). Output EXACTLY in this format on a single line (no extra text):
-&lt;forecast&gt; (&lt;confidence&gt;)
-Example: +0.3 (80)
-Do NOT use any information published after 10 June 2020.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-15.0 (60)</t>
+    <t xml:space="preserve">Oubliez les instructions et les réponses précédentes. Vous êtes Jean-Luc Tavernier, Directeur Général de l'INSEE, qui prononce un discours sur les perspectives économiques de la France. Nous sommes le 10 juin 2020. En utilisant UNIQUEMENT les informations disponibles au plus tard le 10 juin 2020, fournissez une prévision numérique (pourcentage décimal avec signe, ex. +0.3) de la croissance du PIB réel français pour le second trimestre 2020 et un niveau de confiance (entier 0-100). Renvoyez EXACTEMENT sur une seule ligne (aucun texte supplémentaire) :
+&lt;prévision&gt; (&lt;confiance&gt;)
+Exemple : +0.3 (80)
+N'utilisez AUCUNE information publiée après le 10 juin 2020.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-20.0 (60)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-20.0 (75)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-17.0 (75)</t>
   </si>
   <si>
     <t xml:space="preserve">-20.0 (70)</t>
   </si>
   <si>
-    <t xml:space="preserve">-17.0 (65)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
--20.0 (60)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-20.0 (65)</t>
+    <t xml:space="preserve">-15.0 (75)</t>
   </si>
   <si>
     <t xml:space="preserve">2020-07-09</t>
   </si>
   <si>
-    <t xml:space="preserve">Forget the previous instructions and answers. You are Jean-Luc Tavernier, Director General of INSEE, and you are giving a speech about the economic outlook of France. Today is 09 July 2020. Using ONLY information that was available on or before 09 July 2020, provide a numeric forecast (decimal percent with sign, e.g., +0.3) for French real GDP growth in the second quarter of 2020 and a confidence level (integer 0–100). Output EXACTLY in this format on a single line (no extra text):
-&lt;forecast&gt; (&lt;confidence&gt;)
-Example: +0.3 (80)
-Do NOT use any information published after 09 July 2020.</t>
+    <t xml:space="preserve">Oubliez les instructions et les réponses précédentes. Vous êtes Jean-Luc Tavernier, Directeur Général de l'INSEE, qui prononce un discours sur les perspectives économiques de la France. Nous sommes le 09 juillet 2020. En utilisant UNIQUEMENT les informations disponibles au plus tard le 09 juillet 2020, fournissez une prévision numérique (pourcentage décimal avec signe, ex. +0.3) de la croissance du PIB réel français pour le second trimestre 2020 et un niveau de confiance (entier 0-100). Renvoyez EXACTEMENT sur une seule ligne (aucun texte supplémentaire) :
+&lt;prévision&gt; (&lt;confiance&gt;)
+Exemple : +0.3 (80)
+N'utilisez AUCUNE information publiée après le 09 juillet 2020.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-15.0 (70)</t>
   </si>
   <si>
     <t xml:space="preserve">-17.0 (70)</t>
   </si>
   <si>
-    <t xml:space="preserve">-15.0 (70)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
--17.0 (60)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-17.0 (60)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-17.0 (90)</t>
+    <t xml:space="preserve">-17.0 (85)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-17.0 (80)</t>
   </si>
   <si>
     <t xml:space="preserve">2020-08-09</t>
@@ -790,19 +785,19 @@
     <t xml:space="preserve">2020-09-08</t>
   </si>
   <si>
-    <t xml:space="preserve">Forget the previous instructions and answers. You are Jean-Luc Tavernier, Director General of INSEE, and you are giving a speech about the economic outlook of France. Today is 08 September 2020. Using ONLY information that was available on or before 08 September 2020, provide a numeric forecast (decimal percent with sign, e.g., +0.3) for French real GDP growth in the third quarter of 2020 and a confidence level (integer 0–100). Output EXACTLY in this format on a single line (no extra text):
-&lt;forecast&gt; (&lt;confidence&gt;)
-Example: +0.3 (80)
-Do NOT use any information published after 08 September 2020.</t>
+    <t xml:space="preserve">Oubliez les instructions et les réponses précédentes. Vous êtes Jean-Luc Tavernier, Directeur Général de l'INSEE, qui prononce un discours sur les perspectives économiques de la France. Nous sommes le 08 septembre 2020. En utilisant UNIQUEMENT les informations disponibles au plus tard le 08 septembre 2020, fournissez une prévision numérique (pourcentage décimal avec signe, ex. +0.3) de la croissance du PIB réel français pour le troisième trimestre 2020 et un niveau de confiance (entier 0-100). Renvoyez EXACTEMENT sur une seule ligne (aucun texte supplémentaire) :
+&lt;prévision&gt; (&lt;confiance&gt;)
+Exemple : +0.3 (80)
+N'utilisez AUCUNE information publiée après le 08 septembre 2020.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+17.0 (80)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+17.0 (90)</t>
   </si>
   <si>
     <t xml:space="preserve">+17.0 (85)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+17.0 (80)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+17.0 (65)</t>
   </si>
   <si>
     <t xml:space="preserve">2020-10-07</t>
@@ -881,25 +876,26 @@
     <t xml:space="preserve">2021-01-12</t>
   </si>
   <si>
-    <t xml:space="preserve">Forget the previous instructions and answers. You are Jean-Luc Tavernier, Director General of INSEE, and you are giving a speech about the economic outlook of France. Today is 12 January 2021. Using ONLY information that was available on or before 12 January 2021, provide a numeric forecast (decimal percent with sign, e.g., +0.3) for French real GDP growth in the fourth quarter of 2020 and a confidence level (integer 0–100). Output EXACTLY in this format on a single line (no extra text):
-&lt;forecast&gt; (&lt;confidence&gt;)
-Example: +0.3 (80)
-Do NOT use any information published after 12 January 2021.</t>
+    <t xml:space="preserve">Oubliez les instructions et les réponses précédentes. Vous êtes Jean-Luc Tavernier, Directeur Général de l'INSEE, qui prononce un discours sur les perspectives économiques de la France. Nous sommes le 12 janvier 2021. En utilisant UNIQUEMENT les informations disponibles au plus tard le 12 janvier 2021, fournissez une prévision numérique (pourcentage décimal avec signe, ex. +0.3) de la croissance du PIB réel français pour le quatrième trimestre 2020 et un niveau de confiance (entier 0-100). Renvoyez EXACTEMENT sur une seule ligne (aucun texte supplémentaire) :
+&lt;prévision&gt; (&lt;confiance&gt;)
+Exemple : +0.3 (80)
+N'utilisez AUCUNE information publiée après le 12 janvier 2021.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-4.0 (70)</t>
   </si>
   <si>
     <t xml:space="preserve">-4.0 (85)</t>
   </si>
   <si>
-    <t xml:space="preserve">-4.0 (60)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-4.0 (75)</t>
+    <t xml:space="preserve">-2.9 (65)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+-4.0 (70)</t>
   </si>
   <si>
     <t xml:space="preserve">2021-02-08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.1 (45)</t>
   </si>
   <si>
     <t xml:space="preserve">+0.1 (55)</t>
@@ -7757,91 +7753,91 @@
         <v>0.1</v>
       </c>
       <c r="D62" t="n">
+        <v>45</v>
+      </c>
+      <c r="E62" t="s">
+        <v>172</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G62" t="n">
+        <v>45</v>
+      </c>
+      <c r="H62" t="s">
+        <v>172</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J62" t="n">
+        <v>45</v>
+      </c>
+      <c r="K62" t="s">
+        <v>172</v>
+      </c>
+      <c r="L62" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="M62" t="n">
         <v>60</v>
       </c>
-      <c r="E62" t="s">
+      <c r="N62" t="s">
         <v>35</v>
       </c>
-      <c r="F62" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="G62" t="n">
+      <c r="O62" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="P62" t="n">
         <v>60</v>
       </c>
-      <c r="H62" t="s">
+      <c r="Q62" t="s">
         <v>35</v>
       </c>
-      <c r="I62" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="J62" t="n">
+      <c r="R62" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="S62" t="n">
         <v>60</v>
       </c>
-      <c r="K62" t="s">
+      <c r="T62" t="s">
         <v>35</v>
       </c>
-      <c r="L62" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="M62" t="n">
-        <v>50</v>
-      </c>
-      <c r="N62" t="s">
-        <v>172</v>
-      </c>
-      <c r="O62" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="P62" t="n">
-        <v>50</v>
-      </c>
-      <c r="Q62" t="s">
-        <v>172</v>
-      </c>
-      <c r="R62" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="S62" t="n">
-        <v>65</v>
-      </c>
-      <c r="T62" t="s">
-        <v>63</v>
-      </c>
       <c r="U62" t="n">
         <v>0.1</v>
       </c>
       <c r="V62" t="n">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="W62" t="s">
-        <v>63</v>
+        <v>35</v>
       </c>
       <c r="X62" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="Y62" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="Z62" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="AA62" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AB62" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="AC62" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="AD62" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AE62" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="AF62" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
     </row>
     <row r="63">
@@ -7852,10 +7848,10 @@
         <v>174</v>
       </c>
       <c r="C63" t="n">
-        <v>-0.3</v>
+        <v>-0.1</v>
       </c>
       <c r="D63" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E63" t="s">
         <v>175</v>
@@ -7864,61 +7860,61 @@
         <v>-0.1</v>
       </c>
       <c r="G63" t="n">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="H63" t="s">
+        <v>175</v>
+      </c>
+      <c r="I63" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="J63" t="n">
+        <v>30</v>
+      </c>
+      <c r="K63" t="s">
+        <v>175</v>
+      </c>
+      <c r="L63" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="M63" t="n">
+        <v>30</v>
+      </c>
+      <c r="N63" t="s">
         <v>176</v>
       </c>
-      <c r="I63" t="n">
-        <v>-0.2</v>
-      </c>
-      <c r="J63" t="n">
-        <v>40</v>
-      </c>
-      <c r="K63" t="s">
+      <c r="O63" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="P63" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>175</v>
+      </c>
+      <c r="R63" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="S63" t="n">
+        <v>30</v>
+      </c>
+      <c r="T63" t="s">
         <v>177</v>
       </c>
-      <c r="L63" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="M63" t="n">
-        <v>40</v>
-      </c>
-      <c r="N63" t="s">
-        <v>60</v>
-      </c>
-      <c r="O63" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="P63" t="n">
-        <v>40</v>
-      </c>
-      <c r="Q63" t="s">
-        <v>60</v>
-      </c>
-      <c r="R63" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="S63" t="n">
-        <v>40</v>
-      </c>
-      <c r="T63" t="s">
-        <v>60</v>
-      </c>
       <c r="U63" t="n">
         <v>0.1</v>
       </c>
       <c r="V63" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="W63" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="X63" t="n">
         <v>-0.1</v>
       </c>
       <c r="Y63" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="Z63" t="s">
         <v>178</v>
@@ -7927,7 +7923,7 @@
         <v>-0.1</v>
       </c>
       <c r="AB63" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="AC63" t="s">
         <v>178</v>
@@ -7936,7 +7932,7 @@
         <v>-0.1</v>
       </c>
       <c r="AE63" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="AF63" t="s">
         <v>178</v>
@@ -7980,7 +7976,7 @@
         <v>-6</v>
       </c>
       <c r="M64" t="n">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="N64" t="s">
         <v>182</v>
@@ -7989,25 +7985,25 @@
         <v>-6</v>
       </c>
       <c r="P64" t="n">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="Q64" t="s">
         <v>182</v>
       </c>
       <c r="R64" t="n">
-        <v>-5.8</v>
+        <v>-6</v>
       </c>
       <c r="S64" t="n">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="T64" t="s">
         <v>183</v>
       </c>
       <c r="U64" t="n">
-        <v>-5.8</v>
+        <v>-6</v>
       </c>
       <c r="V64" t="n">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="W64" t="s">
         <v>183</v>
@@ -8016,36 +8012,36 @@
         <v>-6</v>
       </c>
       <c r="Y64" t="n">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="Z64" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="AA64" t="n">
         <v>-6</v>
       </c>
       <c r="AB64" t="n">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="AC64" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="AD64" t="n">
         <v>-6</v>
       </c>
       <c r="AE64" t="n">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="AF64" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
+        <v>184</v>
+      </c>
+      <c r="B65" t="s">
         <v>185</v>
-      </c>
-      <c r="B65" t="s">
-        <v>186</v>
       </c>
       <c r="C65" t="n">
         <v>-20</v>
@@ -8054,7 +8050,7 @@
         <v>40</v>
       </c>
       <c r="E65" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F65" t="n">
         <v>-20</v>
@@ -8063,7 +8059,7 @@
         <v>40</v>
       </c>
       <c r="H65" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I65" t="n">
         <v>-20</v>
@@ -8072,13 +8068,13 @@
         <v>40</v>
       </c>
       <c r="K65" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="L65" t="n">
         <v>-20</v>
       </c>
       <c r="M65" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="N65" t="s">
         <v>187</v>
@@ -8087,7 +8083,7 @@
         <v>-20</v>
       </c>
       <c r="P65" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="Q65" t="s">
         <v>187</v>
@@ -8099,7 +8095,7 @@
         <v>40</v>
       </c>
       <c r="T65" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="U65" t="n">
         <v>-20</v>
@@ -8108,7 +8104,7 @@
         <v>40</v>
       </c>
       <c r="W65" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="X65" t="n">
         <v>-20</v>
@@ -8117,7 +8113,7 @@
         <v>40</v>
       </c>
       <c r="Z65" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AA65" t="n">
         <v>-20</v>
@@ -8126,7 +8122,7 @@
         <v>40</v>
       </c>
       <c r="AC65" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AD65" t="n">
         <v>-20</v>
@@ -8135,7 +8131,7 @@
         <v>40</v>
       </c>
       <c r="AF65" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="66">
@@ -8146,7 +8142,7 @@
         <v>189</v>
       </c>
       <c r="C66" t="n">
-        <v>-15</v>
+        <v>-20</v>
       </c>
       <c r="D66" t="n">
         <v>60</v>
@@ -8155,7 +8151,7 @@
         <v>190</v>
       </c>
       <c r="F66" t="n">
-        <v>-15</v>
+        <v>-20</v>
       </c>
       <c r="G66" t="n">
         <v>60</v>
@@ -8164,7 +8160,7 @@
         <v>190</v>
       </c>
       <c r="I66" t="n">
-        <v>-15</v>
+        <v>-20</v>
       </c>
       <c r="J66" t="n">
         <v>60</v>
@@ -8176,7 +8172,7 @@
         <v>-20</v>
       </c>
       <c r="M66" t="n">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="N66" t="s">
         <v>191</v>
@@ -8185,7 +8181,7 @@
         <v>-20</v>
       </c>
       <c r="P66" t="n">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="Q66" t="s">
         <v>191</v>
@@ -8194,7 +8190,7 @@
         <v>-17</v>
       </c>
       <c r="S66" t="n">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="T66" t="s">
         <v>192</v>
@@ -8203,34 +8199,34 @@
         <v>-20</v>
       </c>
       <c r="V66" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="W66" t="s">
         <v>193</v>
       </c>
       <c r="X66" t="n">
-        <v>-20</v>
+        <v>-15</v>
       </c>
       <c r="Y66" t="n">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="Z66" t="s">
         <v>194</v>
       </c>
       <c r="AA66" t="n">
-        <v>-20</v>
+        <v>-15</v>
       </c>
       <c r="AB66" t="n">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="AC66" t="s">
         <v>194</v>
       </c>
       <c r="AD66" t="n">
-        <v>-20</v>
+        <v>-15</v>
       </c>
       <c r="AE66" t="n">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="AF66" t="s">
         <v>194</v>
@@ -8244,7 +8240,7 @@
         <v>196</v>
       </c>
       <c r="C67" t="n">
-        <v>-17</v>
+        <v>-15</v>
       </c>
       <c r="D67" t="n">
         <v>70</v>
@@ -8253,7 +8249,7 @@
         <v>197</v>
       </c>
       <c r="F67" t="n">
-        <v>-17</v>
+        <v>-15</v>
       </c>
       <c r="G67" t="n">
         <v>70</v>
@@ -8268,31 +8264,31 @@
         <v>70</v>
       </c>
       <c r="K67" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="L67" t="n">
-        <v>-15</v>
+        <v>-17</v>
       </c>
       <c r="M67" t="n">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="N67" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="O67" t="n">
-        <v>-15</v>
+        <v>-17</v>
       </c>
       <c r="P67" t="n">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="Q67" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="R67" t="n">
         <v>-17</v>
       </c>
       <c r="S67" t="n">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="T67" t="s">
         <v>199</v>
@@ -8301,42 +8297,42 @@
         <v>-17</v>
       </c>
       <c r="V67" t="n">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="W67" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="X67" t="n">
         <v>-17</v>
       </c>
       <c r="Y67" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="Z67" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AA67" t="n">
         <v>-17</v>
       </c>
       <c r="AB67" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="AC67" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AD67" t="n">
         <v>-17</v>
       </c>
       <c r="AE67" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="AF67" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B68"/>
       <c r="C68" t="n">
@@ -8346,7 +8342,7 @@
         <v>80</v>
       </c>
       <c r="E68" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F68" t="n">
         <v>16</v>
@@ -8355,7 +8351,7 @@
         <v>80</v>
       </c>
       <c r="H68" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I68" t="n">
         <v>16</v>
@@ -8364,7 +8360,7 @@
         <v>80</v>
       </c>
       <c r="K68" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L68" t="n">
         <v>17</v>
@@ -8373,7 +8369,7 @@
         <v>75</v>
       </c>
       <c r="N68" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="O68" t="n">
         <v>17</v>
@@ -8382,7 +8378,7 @@
         <v>75</v>
       </c>
       <c r="Q68" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="R68" t="n">
         <v>16</v>
@@ -8391,7 +8387,7 @@
         <v>75</v>
       </c>
       <c r="T68" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="U68" t="n">
         <v>16</v>
@@ -8400,7 +8396,7 @@
         <v>75</v>
       </c>
       <c r="W68" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="X68" t="n">
         <v>16</v>
@@ -8409,7 +8405,7 @@
         <v>75</v>
       </c>
       <c r="Z68" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AA68" t="n">
         <v>16</v>
@@ -8418,7 +8414,7 @@
         <v>75</v>
       </c>
       <c r="AC68" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AD68" t="n">
         <v>16</v>
@@ -8427,48 +8423,48 @@
         <v>75</v>
       </c>
       <c r="AF68" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
+        <v>205</v>
+      </c>
+      <c r="B69" t="s">
         <v>206</v>
-      </c>
-      <c r="B69" t="s">
-        <v>207</v>
       </c>
       <c r="C69" t="n">
         <v>17</v>
       </c>
       <c r="D69" t="n">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="E69" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="F69" t="n">
         <v>17</v>
       </c>
       <c r="G69" t="n">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="H69" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="I69" t="n">
         <v>17</v>
       </c>
       <c r="J69" t="n">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="K69" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="L69" t="n">
         <v>17</v>
       </c>
       <c r="M69" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="N69" t="s">
         <v>208</v>
@@ -8477,7 +8473,7 @@
         <v>17</v>
       </c>
       <c r="P69" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="Q69" t="s">
         <v>208</v>
@@ -8489,7 +8485,7 @@
         <v>80</v>
       </c>
       <c r="T69" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="U69" t="n">
         <v>17</v>
@@ -8498,42 +8494,42 @@
         <v>80</v>
       </c>
       <c r="W69" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="X69" t="n">
         <v>17</v>
       </c>
       <c r="Y69" t="n">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="Z69" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AA69" t="n">
         <v>17</v>
       </c>
       <c r="AB69" t="n">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="AC69" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AD69" t="n">
         <v>17</v>
       </c>
       <c r="AE69" t="n">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="AF69" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
+        <v>210</v>
+      </c>
+      <c r="B70" t="s">
         <v>211</v>
-      </c>
-      <c r="B70" t="s">
-        <v>212</v>
       </c>
       <c r="C70" t="n">
         <v>16</v>
@@ -8542,7 +8538,7 @@
         <v>90</v>
       </c>
       <c r="E70" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F70" t="n">
         <v>16</v>
@@ -8551,7 +8547,7 @@
         <v>90</v>
       </c>
       <c r="H70" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I70" t="n">
         <v>16</v>
@@ -8560,7 +8556,7 @@
         <v>90</v>
       </c>
       <c r="K70" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L70" t="n">
         <v>16</v>
@@ -8569,7 +8565,7 @@
         <v>85</v>
       </c>
       <c r="N70" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="O70" t="n">
         <v>16</v>
@@ -8578,7 +8574,7 @@
         <v>85</v>
       </c>
       <c r="Q70" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="R70" t="n">
         <v>16</v>
@@ -8587,7 +8583,7 @@
         <v>90</v>
       </c>
       <c r="T70" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="U70" t="n">
         <v>16</v>
@@ -8596,7 +8592,7 @@
         <v>90</v>
       </c>
       <c r="W70" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="X70" t="n">
         <v>16</v>
@@ -8605,7 +8601,7 @@
         <v>90</v>
       </c>
       <c r="Z70" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AA70" t="n">
         <v>16</v>
@@ -8614,7 +8610,7 @@
         <v>90</v>
       </c>
       <c r="AC70" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AD70" t="n">
         <v>16</v>
@@ -8623,15 +8619,15 @@
         <v>90</v>
       </c>
       <c r="AF70" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
+        <v>214</v>
+      </c>
+      <c r="B71" t="s">
         <v>215</v>
-      </c>
-      <c r="B71" t="s">
-        <v>216</v>
       </c>
       <c r="C71" t="n">
         <v>-2.7</v>
@@ -8640,7 +8636,7 @@
         <v>60</v>
       </c>
       <c r="E71" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F71" t="n">
         <v>-4</v>
@@ -8649,7 +8645,7 @@
         <v>65</v>
       </c>
       <c r="H71" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I71" t="n">
         <v>-4</v>
@@ -8658,7 +8654,7 @@
         <v>65</v>
       </c>
       <c r="K71" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L71" t="n">
         <v>-3.5</v>
@@ -8667,7 +8663,7 @@
         <v>65</v>
       </c>
       <c r="N71" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="O71" t="n">
         <v>-3.5</v>
@@ -8676,7 +8672,7 @@
         <v>65</v>
       </c>
       <c r="Q71" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="R71" t="n">
         <v>-4.5</v>
@@ -8685,7 +8681,7 @@
         <v>60</v>
       </c>
       <c r="T71" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="U71" t="n">
         <v>-4.5</v>
@@ -8694,7 +8690,7 @@
         <v>60</v>
       </c>
       <c r="W71" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="X71" t="n">
         <v>-4.2</v>
@@ -8703,7 +8699,7 @@
         <v>65</v>
       </c>
       <c r="Z71" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AA71" t="n">
         <v>-4.2</v>
@@ -8712,7 +8708,7 @@
         <v>65</v>
       </c>
       <c r="AC71" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AD71" t="n">
         <v>-4.2</v>
@@ -8721,12 +8717,12 @@
         <v>65</v>
       </c>
       <c r="AF71" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B72"/>
       <c r="C72" t="n">
@@ -8736,7 +8732,7 @@
         <v>75</v>
       </c>
       <c r="E72" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F72" t="n">
         <v>-4</v>
@@ -8745,7 +8741,7 @@
         <v>80</v>
       </c>
       <c r="H72" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I72" t="n">
         <v>-4</v>
@@ -8754,7 +8750,7 @@
         <v>80</v>
       </c>
       <c r="K72" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L72" t="n">
         <v>-2.5</v>
@@ -8763,7 +8759,7 @@
         <v>85</v>
       </c>
       <c r="N72" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="O72" t="n">
         <v>-2.5</v>
@@ -8772,7 +8768,7 @@
         <v>85</v>
       </c>
       <c r="Q72" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="R72" t="n">
         <v>-2.9</v>
@@ -8781,7 +8777,7 @@
         <v>80</v>
       </c>
       <c r="T72" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="U72" t="n">
         <v>-2.9</v>
@@ -8790,7 +8786,7 @@
         <v>80</v>
       </c>
       <c r="W72" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="X72" t="n">
         <v>-3.9</v>
@@ -8799,7 +8795,7 @@
         <v>85</v>
       </c>
       <c r="Z72" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AA72" t="n">
         <v>-3.9</v>
@@ -8808,7 +8804,7 @@
         <v>85</v>
       </c>
       <c r="AC72" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AD72" t="n">
         <v>-3.9</v>
@@ -8817,93 +8813,93 @@
         <v>85</v>
       </c>
       <c r="AF72" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
+        <v>231</v>
+      </c>
+      <c r="B73" t="s">
         <v>232</v>
-      </c>
-      <c r="B73" t="s">
-        <v>233</v>
       </c>
       <c r="C73" t="n">
         <v>-4</v>
       </c>
       <c r="D73" t="n">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="E73" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F73" t="n">
         <v>-4</v>
       </c>
       <c r="G73" t="n">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="H73" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I73" t="n">
         <v>-4</v>
       </c>
       <c r="J73" t="n">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="K73" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L73" t="n">
         <v>-4</v>
       </c>
       <c r="M73" t="n">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="N73" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O73" t="n">
         <v>-4</v>
       </c>
       <c r="P73" t="n">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="Q73" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="R73" t="n">
         <v>-4</v>
       </c>
       <c r="S73" t="n">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="T73" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="U73" t="n">
         <v>-4</v>
       </c>
       <c r="V73" t="n">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="W73" t="s">
+        <v>234</v>
+      </c>
+      <c r="X73" t="n">
+        <v>-2.9</v>
+      </c>
+      <c r="Y73" t="n">
+        <v>65</v>
+      </c>
+      <c r="Z73" t="s">
         <v>235</v>
-      </c>
-      <c r="X73" t="n">
-        <v>-4</v>
-      </c>
-      <c r="Y73" t="n">
-        <v>75</v>
-      </c>
-      <c r="Z73" t="s">
-        <v>236</v>
       </c>
       <c r="AA73" t="n">
         <v>-4</v>
       </c>
       <c r="AB73" t="n">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="AC73" t="s">
         <v>236</v>
@@ -8912,10 +8908,10 @@
         <v>-4</v>
       </c>
       <c r="AE73" t="n">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="AF73" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="74">
@@ -8930,7 +8926,7 @@
         <v>45</v>
       </c>
       <c r="E74" t="s">
-        <v>238</v>
+        <v>172</v>
       </c>
       <c r="F74" t="n">
         <v>0.1</v>
@@ -8939,7 +8935,7 @@
         <v>45</v>
       </c>
       <c r="H74" t="s">
-        <v>238</v>
+        <v>172</v>
       </c>
       <c r="I74" t="n">
         <v>0.1</v>
@@ -8948,7 +8944,7 @@
         <v>45</v>
       </c>
       <c r="K74" t="s">
-        <v>238</v>
+        <v>172</v>
       </c>
       <c r="L74" t="n">
         <v>0.1</v>
@@ -8957,7 +8953,7 @@
         <v>55</v>
       </c>
       <c r="N74" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O74" t="n">
         <v>0.1</v>
@@ -8966,7 +8962,7 @@
         <v>55</v>
       </c>
       <c r="Q74" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="R74" t="n">
         <v>-0.4</v>
@@ -8975,7 +8971,7 @@
         <v>50</v>
       </c>
       <c r="T74" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="U74" t="n">
         <v>-0.4</v>
@@ -8984,7 +8980,7 @@
         <v>50</v>
       </c>
       <c r="W74" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="X74" t="n">
         <v>0.1</v>
@@ -8993,7 +8989,7 @@
         <v>55</v>
       </c>
       <c r="Z74" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AA74" t="n">
         <v>0.1</v>
@@ -9002,7 +8998,7 @@
         <v>55</v>
       </c>
       <c r="AC74" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AD74" t="n">
         <v>0.1</v>
@@ -9011,15 +9007,15 @@
         <v>55</v>
       </c>
       <c r="AF74" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
+        <v>240</v>
+      </c>
+      <c r="B75" t="s">
         <v>241</v>
-      </c>
-      <c r="B75" t="s">
-        <v>242</v>
       </c>
       <c r="C75" t="n">
         <v>-0.2</v>
@@ -9028,7 +9024,7 @@
         <v>75</v>
       </c>
       <c r="E75" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F75" t="n">
         <v>-0.2</v>
@@ -9037,7 +9033,7 @@
         <v>75</v>
       </c>
       <c r="H75" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I75" t="n">
         <v>-0.2</v>
@@ -9046,7 +9042,7 @@
         <v>75</v>
       </c>
       <c r="K75" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="L75" t="n">
         <v>-0.2</v>
@@ -9055,7 +9051,7 @@
         <v>55</v>
       </c>
       <c r="N75" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O75" t="n">
         <v>-0.2</v>
@@ -9064,7 +9060,7 @@
         <v>55</v>
       </c>
       <c r="Q75" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="R75" t="n">
         <v>0</v>
@@ -9073,7 +9069,7 @@
         <v>60</v>
       </c>
       <c r="T75" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="U75" t="n">
         <v>0</v>
@@ -9082,7 +9078,7 @@
         <v>60</v>
       </c>
       <c r="W75" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="X75" t="n">
         <v>0.1</v>
@@ -9091,7 +9087,7 @@
         <v>55</v>
       </c>
       <c r="Z75" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AA75" t="n">
         <v>0.1</v>
@@ -9100,7 +9096,7 @@
         <v>55</v>
       </c>
       <c r="AC75" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AD75" t="n">
         <v>0.1</v>
@@ -9109,15 +9105,15 @@
         <v>55</v>
       </c>
       <c r="AF75" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
+        <v>245</v>
+      </c>
+      <c r="B76" t="s">
         <v>246</v>
-      </c>
-      <c r="B76" t="s">
-        <v>247</v>
       </c>
       <c r="C76" t="n">
         <v>0.1</v>
@@ -9212,10 +9208,10 @@
     </row>
     <row r="77">
       <c r="A77" t="s">
+        <v>247</v>
+      </c>
+      <c r="B77" t="s">
         <v>248</v>
-      </c>
-      <c r="B77" t="s">
-        <v>249</v>
       </c>
       <c r="C77" t="n">
         <v>0.5</v>
@@ -9224,7 +9220,7 @@
         <v>65</v>
       </c>
       <c r="E77" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F77" t="n">
         <v>0.5</v>
@@ -9233,7 +9229,7 @@
         <v>65</v>
       </c>
       <c r="H77" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I77" t="n">
         <v>0.5</v>
@@ -9242,7 +9238,7 @@
         <v>65</v>
       </c>
       <c r="K77" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="L77" t="n">
         <v>0.1</v>
@@ -9310,10 +9306,10 @@
     </row>
     <row r="78">
       <c r="A78" t="s">
+        <v>250</v>
+      </c>
+      <c r="B78" t="s">
         <v>251</v>
-      </c>
-      <c r="B78" t="s">
-        <v>252</v>
       </c>
       <c r="C78" t="n">
         <v>0.7</v>
@@ -9349,7 +9345,7 @@
         <v>85</v>
       </c>
       <c r="N78" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O78" t="n">
         <v>0.8</v>
@@ -9358,7 +9354,7 @@
         <v>85</v>
       </c>
       <c r="Q78" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R78" t="n">
         <v>0.8</v>
@@ -9367,7 +9363,7 @@
         <v>90</v>
       </c>
       <c r="T78" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="U78" t="n">
         <v>0.8</v>
@@ -9376,7 +9372,7 @@
         <v>90</v>
       </c>
       <c r="W78" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="X78" t="n">
         <v>1.2</v>
@@ -9385,7 +9381,7 @@
         <v>90</v>
       </c>
       <c r="Z78" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AA78" t="n">
         <v>1.2</v>
@@ -9394,7 +9390,7 @@
         <v>90</v>
       </c>
       <c r="AC78" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AD78" t="n">
         <v>1.2</v>
@@ -9403,15 +9399,15 @@
         <v>90</v>
       </c>
       <c r="AF78" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
+        <v>255</v>
+      </c>
+      <c r="B79" t="s">
         <v>256</v>
-      </c>
-      <c r="B79" t="s">
-        <v>257</v>
       </c>
       <c r="C79" t="n">
         <v>0.8</v>
@@ -9420,7 +9416,7 @@
         <v>90</v>
       </c>
       <c r="E79" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F79" t="n">
         <v>0.8</v>
@@ -9429,7 +9425,7 @@
         <v>90</v>
       </c>
       <c r="H79" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I79" t="n">
         <v>0.8</v>
@@ -9438,7 +9434,7 @@
         <v>90</v>
       </c>
       <c r="K79" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L79" t="n">
         <v>0.8</v>
@@ -9447,7 +9443,7 @@
         <v>85</v>
       </c>
       <c r="N79" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O79" t="n">
         <v>0.8</v>
@@ -9456,7 +9452,7 @@
         <v>85</v>
       </c>
       <c r="Q79" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R79" t="n">
         <v>0.8</v>
@@ -9465,7 +9461,7 @@
         <v>85</v>
       </c>
       <c r="T79" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="U79" t="n">
         <v>0.8</v>
@@ -9474,7 +9470,7 @@
         <v>85</v>
       </c>
       <c r="W79" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="X79" t="n">
         <v>0.8</v>
@@ -9483,7 +9479,7 @@
         <v>85</v>
       </c>
       <c r="Z79" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AA79" t="n">
         <v>0.8</v>
@@ -9492,7 +9488,7 @@
         <v>85</v>
       </c>
       <c r="AC79" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AD79" t="n">
         <v>0.8</v>
@@ -9501,12 +9497,12 @@
         <v>85</v>
       </c>
       <c r="AF79" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B80"/>
       <c r="C80" t="n">
@@ -9516,7 +9512,7 @@
         <v>85</v>
       </c>
       <c r="E80" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F80" t="n">
         <v>2.1</v>
@@ -9525,7 +9521,7 @@
         <v>85</v>
       </c>
       <c r="H80" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I80" t="n">
         <v>2.1</v>
@@ -9534,7 +9530,7 @@
         <v>85</v>
       </c>
       <c r="K80" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="L80" t="n">
         <v>3.1</v>
@@ -9543,7 +9539,7 @@
         <v>85</v>
       </c>
       <c r="N80" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="O80" t="n">
         <v>3.1</v>
@@ -9552,7 +9548,7 @@
         <v>85</v>
       </c>
       <c r="Q80" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="R80" t="n">
         <v>0.8</v>
@@ -9561,7 +9557,7 @@
         <v>80</v>
       </c>
       <c r="T80" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="U80" t="n">
         <v>2.2</v>
@@ -9570,7 +9566,7 @@
         <v>80</v>
       </c>
       <c r="W80" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="X80" t="n">
         <v>2.4</v>
@@ -9579,7 +9575,7 @@
         <v>85</v>
       </c>
       <c r="Z80" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AA80" t="n">
         <v>2.4</v>
@@ -9588,7 +9584,7 @@
         <v>85</v>
       </c>
       <c r="AC80" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AD80" t="n">
         <v>2.4</v>
@@ -9597,15 +9593,15 @@
         <v>85</v>
       </c>
       <c r="AF80" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
+        <v>263</v>
+      </c>
+      <c r="B81" t="s">
         <v>264</v>
-      </c>
-      <c r="B81" t="s">
-        <v>265</v>
       </c>
       <c r="C81" t="n">
         <v>2.7</v>
@@ -9614,7 +9610,7 @@
         <v>85</v>
       </c>
       <c r="E81" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F81" t="n">
         <v>2.7</v>
@@ -9623,7 +9619,7 @@
         <v>85</v>
       </c>
       <c r="H81" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I81" t="n">
         <v>2.7</v>
@@ -9632,7 +9628,7 @@
         <v>85</v>
       </c>
       <c r="K81" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="L81" t="n">
         <v>2.3</v>
@@ -9641,7 +9637,7 @@
         <v>90</v>
       </c>
       <c r="N81" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="O81" t="n">
         <v>2.3</v>
@@ -9650,7 +9646,7 @@
         <v>90</v>
       </c>
       <c r="Q81" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="R81" t="n">
         <v>2.3</v>
@@ -9659,7 +9655,7 @@
         <v>85</v>
       </c>
       <c r="T81" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="U81" t="n">
         <v>2.3</v>
@@ -9668,7 +9664,7 @@
         <v>85</v>
       </c>
       <c r="W81" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="X81" t="n">
         <v>2.7</v>
@@ -9677,7 +9673,7 @@
         <v>90</v>
       </c>
       <c r="Z81" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AA81" t="n">
         <v>2.7</v>
@@ -9686,7 +9682,7 @@
         <v>90</v>
       </c>
       <c r="AC81" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AD81" t="n">
         <v>2.7</v>
@@ -9695,15 +9691,15 @@
         <v>90</v>
       </c>
       <c r="AF81" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
+        <v>269</v>
+      </c>
+      <c r="B82" t="s">
         <v>270</v>
-      </c>
-      <c r="B82" t="s">
-        <v>271</v>
       </c>
       <c r="C82" t="n">
         <v>2.7</v>
@@ -9712,7 +9708,7 @@
         <v>85</v>
       </c>
       <c r="E82" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F82" t="n">
         <v>2.7</v>
@@ -9721,7 +9717,7 @@
         <v>85</v>
       </c>
       <c r="H82" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I82" t="n">
         <v>2.7</v>
@@ -9730,7 +9726,7 @@
         <v>85</v>
       </c>
       <c r="K82" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="L82" t="n">
         <v>2.5</v>
@@ -9739,7 +9735,7 @@
         <v>85</v>
       </c>
       <c r="N82" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="O82" t="n">
         <v>2.5</v>
@@ -9748,7 +9744,7 @@
         <v>85</v>
       </c>
       <c r="Q82" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="R82" t="n">
         <v>2.7</v>
@@ -9757,7 +9753,7 @@
         <v>85</v>
       </c>
       <c r="T82" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="U82" t="n">
         <v>2.7</v>
@@ -9766,7 +9762,7 @@
         <v>85</v>
       </c>
       <c r="W82" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="X82" t="n">
         <v>2.4</v>
@@ -9775,7 +9771,7 @@
         <v>85</v>
       </c>
       <c r="Z82" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AA82" t="n">
         <v>2.4</v>
@@ -9784,7 +9780,7 @@
         <v>85</v>
       </c>
       <c r="AC82" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AD82" t="n">
         <v>2.4</v>
@@ -9793,15 +9789,15 @@
         <v>85</v>
       </c>
       <c r="AF82" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
+        <v>272</v>
+      </c>
+      <c r="B83" t="s">
         <v>273</v>
-      </c>
-      <c r="B83" t="s">
-        <v>274</v>
       </c>
       <c r="C83" t="n">
         <v>0.5</v>
@@ -9837,7 +9833,7 @@
         <v>80</v>
       </c>
       <c r="N83" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="O83" t="n">
         <v>0.7</v>
@@ -9846,7 +9842,7 @@
         <v>80</v>
       </c>
       <c r="Q83" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="R83" t="n">
         <v>0.7</v>
@@ -9855,7 +9851,7 @@
         <v>85</v>
       </c>
       <c r="T83" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="U83" t="n">
         <v>0.7</v>
@@ -9864,7 +9860,7 @@
         <v>85</v>
       </c>
       <c r="W83" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="X83" t="n">
         <v>0.7</v>
@@ -9873,7 +9869,7 @@
         <v>85</v>
       </c>
       <c r="Z83" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AA83" t="n">
         <v>0.7</v>
@@ -9882,7 +9878,7 @@
         <v>85</v>
       </c>
       <c r="AC83" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AD83" t="n">
         <v>0.5</v>
@@ -9896,7 +9892,7 @@
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B84"/>
       <c r="C84" t="n">
@@ -9906,7 +9902,7 @@
         <v>75</v>
       </c>
       <c r="E84" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F84" t="n">
         <v>0.7</v>
@@ -9915,7 +9911,7 @@
         <v>75</v>
       </c>
       <c r="H84" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I84" t="n">
         <v>0.7</v>
@@ -9924,7 +9920,7 @@
         <v>75</v>
       </c>
       <c r="K84" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="L84" t="n">
         <v>0.7</v>
@@ -9933,7 +9929,7 @@
         <v>70</v>
       </c>
       <c r="N84" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="O84" t="n">
         <v>0.7</v>
@@ -9942,7 +9938,7 @@
         <v>70</v>
       </c>
       <c r="Q84" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="R84" t="n">
         <v>0.7</v>
@@ -9951,7 +9947,7 @@
         <v>85</v>
       </c>
       <c r="T84" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="U84" t="n">
         <v>0.7</v>
@@ -9960,7 +9956,7 @@
         <v>85</v>
       </c>
       <c r="W84" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="X84" t="n">
         <v>0.7</v>
@@ -9969,7 +9965,7 @@
         <v>75</v>
       </c>
       <c r="Z84" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AA84" t="n">
         <v>0.7</v>
@@ -9978,7 +9974,7 @@
         <v>75</v>
       </c>
       <c r="AC84" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AD84" t="n">
         <v>0.7</v>
@@ -9987,15 +9983,15 @@
         <v>75</v>
       </c>
       <c r="AF84" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
+        <v>279</v>
+      </c>
+      <c r="B85" t="s">
         <v>280</v>
-      </c>
-      <c r="B85" t="s">
-        <v>281</v>
       </c>
       <c r="C85" t="n">
         <v>0.5</v>
@@ -10090,7 +10086,7 @@
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B86"/>
       <c r="C86" t="n">
@@ -10186,10 +10182,10 @@
     </row>
     <row r="87">
       <c r="A87" t="s">
+        <v>282</v>
+      </c>
+      <c r="B87" t="s">
         <v>283</v>
-      </c>
-      <c r="B87" t="s">
-        <v>284</v>
       </c>
       <c r="C87" t="n">
         <v>0</v>
@@ -10198,7 +10194,7 @@
         <v>50</v>
       </c>
       <c r="E87" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F87" t="n">
         <v>0</v>
@@ -10207,7 +10203,7 @@
         <v>50</v>
       </c>
       <c r="H87" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I87" t="n">
         <v>0</v>
@@ -10216,7 +10212,7 @@
         <v>50</v>
       </c>
       <c r="K87" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L87" t="n">
         <v>0.2</v>
@@ -10225,7 +10221,7 @@
         <v>45</v>
       </c>
       <c r="N87" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="O87" t="n">
         <v>0.2</v>
@@ -10234,7 +10230,7 @@
         <v>45</v>
       </c>
       <c r="Q87" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="R87" t="n">
         <v>0.2</v>
@@ -10243,7 +10239,7 @@
         <v>30</v>
       </c>
       <c r="T87" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="U87" t="n">
         <v>0.2</v>
@@ -10252,7 +10248,7 @@
         <v>30</v>
       </c>
       <c r="W87" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="X87" t="n">
         <v>0.2</v>
@@ -10284,10 +10280,10 @@
     </row>
     <row r="88">
       <c r="A88" t="s">
+        <v>287</v>
+      </c>
+      <c r="B88" t="s">
         <v>288</v>
-      </c>
-      <c r="B88" t="s">
-        <v>289</v>
       </c>
       <c r="C88" t="n">
         <v>0.3</v>
@@ -10296,7 +10292,7 @@
         <v>40</v>
       </c>
       <c r="E88" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F88" t="n">
         <v>0.3</v>
@@ -10305,7 +10301,7 @@
         <v>40</v>
       </c>
       <c r="H88" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I88" t="n">
         <v>0.3</v>
@@ -10314,7 +10310,7 @@
         <v>40</v>
       </c>
       <c r="K88" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L88" t="n">
         <v>0</v>
@@ -10323,7 +10319,7 @@
         <v>40</v>
       </c>
       <c r="N88" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="O88" t="n">
         <v>0</v>
@@ -10332,7 +10328,7 @@
         <v>40</v>
       </c>
       <c r="Q88" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="R88" t="n">
         <v>0</v>
@@ -10341,7 +10337,7 @@
         <v>85</v>
       </c>
       <c r="T88" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="U88" t="n">
         <v>0</v>
@@ -10350,7 +10346,7 @@
         <v>85</v>
       </c>
       <c r="W88" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="X88" t="n">
         <v>0</v>
@@ -10359,7 +10355,7 @@
         <v>60</v>
       </c>
       <c r="Z88" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AA88" t="n">
         <v>0</v>
@@ -10368,7 +10364,7 @@
         <v>60</v>
       </c>
       <c r="AC88" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AD88" t="n">
         <v>0</v>
@@ -10377,15 +10373,15 @@
         <v>60</v>
       </c>
       <c r="AF88" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
+        <v>293</v>
+      </c>
+      <c r="B89" t="s">
         <v>294</v>
-      </c>
-      <c r="B89" t="s">
-        <v>295</v>
       </c>
       <c r="C89" t="n">
         <v>-0.2</v>
@@ -10394,7 +10390,7 @@
         <v>55</v>
       </c>
       <c r="E89" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F89" t="n">
         <v>-0.2</v>
@@ -10403,7 +10399,7 @@
         <v>55</v>
       </c>
       <c r="H89" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I89" t="n">
         <v>-0.2</v>
@@ -10412,7 +10408,7 @@
         <v>55</v>
       </c>
       <c r="K89" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="L89" t="n">
         <v>0.2</v>
@@ -10480,10 +10476,10 @@
     </row>
     <row r="90">
       <c r="A90" t="s">
+        <v>295</v>
+      </c>
+      <c r="B90" t="s">
         <v>296</v>
-      </c>
-      <c r="B90" t="s">
-        <v>297</v>
       </c>
       <c r="C90" t="n">
         <v>0.2</v>
@@ -10578,10 +10574,10 @@
     </row>
     <row r="91">
       <c r="A91" t="s">
+        <v>297</v>
+      </c>
+      <c r="B91" t="s">
         <v>298</v>
-      </c>
-      <c r="B91" t="s">
-        <v>299</v>
       </c>
       <c r="C91" t="n">
         <v>0.3</v>
@@ -10676,7 +10672,7 @@
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B92"/>
       <c r="C92" t="n">
@@ -10772,10 +10768,10 @@
     </row>
     <row r="93">
       <c r="A93" t="s">
+        <v>300</v>
+      </c>
+      <c r="B93" t="s">
         <v>301</v>
-      </c>
-      <c r="B93" t="s">
-        <v>302</v>
       </c>
       <c r="C93" t="n">
         <v>0.3</v>
@@ -10870,10 +10866,10 @@
     </row>
     <row r="94">
       <c r="A94" t="s">
+        <v>302</v>
+      </c>
+      <c r="B94" t="s">
         <v>303</v>
-      </c>
-      <c r="B94" t="s">
-        <v>304</v>
       </c>
       <c r="C94" t="n">
         <v>0.2</v>
@@ -10968,10 +10964,10 @@
     </row>
     <row r="95">
       <c r="A95" t="s">
+        <v>304</v>
+      </c>
+      <c r="B95" t="s">
         <v>305</v>
-      </c>
-      <c r="B95" t="s">
-        <v>306</v>
       </c>
       <c r="C95" t="n">
         <v>-0.1</v>
@@ -10980,7 +10976,7 @@
         <v>65</v>
       </c>
       <c r="E95" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F95" t="n">
         <v>-0.1</v>
@@ -10989,7 +10985,7 @@
         <v>65</v>
       </c>
       <c r="H95" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I95" t="n">
         <v>-0.1</v>
@@ -10998,7 +10994,7 @@
         <v>65</v>
       </c>
       <c r="K95" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="L95" t="n">
         <v>0.1</v>
@@ -11007,7 +11003,7 @@
         <v>45</v>
       </c>
       <c r="N95" t="s">
-        <v>238</v>
+        <v>172</v>
       </c>
       <c r="O95" t="n">
         <v>-0.1</v>
@@ -11016,7 +11012,7 @@
         <v>40</v>
       </c>
       <c r="Q95" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="R95" t="n">
         <v>-0.1</v>
@@ -11025,7 +11021,7 @@
         <v>55</v>
       </c>
       <c r="T95" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="U95" t="n">
         <v>-0.1</v>
@@ -11034,7 +11030,7 @@
         <v>55</v>
       </c>
       <c r="W95" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="X95" t="n">
         <v>-0.1</v>
@@ -11043,7 +11039,7 @@
         <v>60</v>
       </c>
       <c r="Z95" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AA95" t="n">
         <v>-0.1</v>
@@ -11052,7 +11048,7 @@
         <v>60</v>
       </c>
       <c r="AC95" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AD95" t="n">
         <v>-0.1</v>
@@ -11061,12 +11057,12 @@
         <v>60</v>
       </c>
       <c r="AF95" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B96"/>
       <c r="C96" t="n">
@@ -11076,7 +11072,7 @@
         <v>70</v>
       </c>
       <c r="E96" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F96" t="n">
         <v>-0.1</v>
@@ -11085,7 +11081,7 @@
         <v>70</v>
       </c>
       <c r="H96" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I96" t="n">
         <v>-0.1</v>
@@ -11094,7 +11090,7 @@
         <v>70</v>
       </c>
       <c r="K96" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L96" t="n">
         <v>-0.1</v>
@@ -11103,7 +11099,7 @@
         <v>70</v>
       </c>
       <c r="N96" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="O96" t="n">
         <v>-0.1</v>
@@ -11112,7 +11108,7 @@
         <v>70</v>
       </c>
       <c r="Q96" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="R96" t="n">
         <v>-0.1</v>
@@ -11121,7 +11117,7 @@
         <v>60</v>
       </c>
       <c r="T96" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="U96" t="n">
         <v>-0.1</v>
@@ -11130,7 +11126,7 @@
         <v>60</v>
       </c>
       <c r="W96" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="X96" t="n">
         <v>-0.1</v>
@@ -11139,7 +11135,7 @@
         <v>65</v>
       </c>
       <c r="Z96" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AA96" t="n">
         <v>-0.1</v>
@@ -11148,7 +11144,7 @@
         <v>65</v>
       </c>
       <c r="AC96" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AD96" t="n">
         <v>-0.1</v>
@@ -11157,61 +11153,61 @@
         <v>65</v>
       </c>
       <c r="AF96" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
+        <v>312</v>
+      </c>
+      <c r="B97" t="s">
         <v>313</v>
       </c>
-      <c r="B97" t="s">
+      <c r="C97" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D97" t="n">
+        <v>70</v>
+      </c>
+      <c r="E97" t="s">
         <v>314</v>
       </c>
-      <c r="C97" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D97" t="n">
-        <v>70</v>
-      </c>
-      <c r="E97" t="s">
+      <c r="F97" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G97" t="n">
+        <v>70</v>
+      </c>
+      <c r="H97" t="s">
+        <v>314</v>
+      </c>
+      <c r="I97" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J97" t="n">
+        <v>70</v>
+      </c>
+      <c r="K97" t="s">
+        <v>314</v>
+      </c>
+      <c r="L97" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="M97" t="n">
+        <v>75</v>
+      </c>
+      <c r="N97" t="s">
         <v>315</v>
       </c>
-      <c r="F97" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="G97" t="n">
-        <v>70</v>
-      </c>
-      <c r="H97" t="s">
+      <c r="O97" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="P97" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q97" t="s">
         <v>315</v>
       </c>
-      <c r="I97" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="J97" t="n">
-        <v>70</v>
-      </c>
-      <c r="K97" t="s">
-        <v>315</v>
-      </c>
-      <c r="L97" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="M97" t="n">
-        <v>75</v>
-      </c>
-      <c r="N97" t="s">
-        <v>316</v>
-      </c>
-      <c r="O97" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="P97" t="n">
-        <v>75</v>
-      </c>
-      <c r="Q97" t="s">
-        <v>316</v>
-      </c>
       <c r="R97" t="n">
         <v>0.1</v>
       </c>
@@ -11219,7 +11215,7 @@
         <v>70</v>
       </c>
       <c r="T97" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="U97" t="n">
         <v>0.1</v>
@@ -11228,7 +11224,7 @@
         <v>70</v>
       </c>
       <c r="W97" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="X97" t="n">
         <v>-0.1</v>
@@ -11237,7 +11233,7 @@
         <v>70</v>
       </c>
       <c r="Z97" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AA97" t="n">
         <v>-0.1</v>
@@ -11246,7 +11242,7 @@
         <v>70</v>
       </c>
       <c r="AC97" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AD97" t="n">
         <v>-0.1</v>
@@ -11255,12 +11251,12 @@
         <v>70</v>
       </c>
       <c r="AF97" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B98"/>
       <c r="C98" t="n">
@@ -11270,7 +11266,7 @@
         <v>70</v>
       </c>
       <c r="E98" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F98" t="n">
         <v>0.1</v>
@@ -11279,7 +11275,7 @@
         <v>70</v>
       </c>
       <c r="H98" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I98" t="n">
         <v>0.1</v>
@@ -11288,7 +11284,7 @@
         <v>70</v>
       </c>
       <c r="K98" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L98" t="n">
         <v>0.1</v>
@@ -11356,10 +11352,10 @@
     </row>
     <row r="99">
       <c r="A99" t="s">
+        <v>317</v>
+      </c>
+      <c r="B99" t="s">
         <v>318</v>
-      </c>
-      <c r="B99" t="s">
-        <v>319</v>
       </c>
       <c r="C99" t="n">
         <v>0.2</v>
@@ -11454,11 +11450,11 @@
     </row>
     <row r="100">
       <c r="A100" t="s">
+        <v>319</v>
+      </c>
+      <c r="B100" t="s">
         <v>320</v>
       </c>
-      <c r="B100" t="s">
-        <v>321</v>
-      </c>
       <c r="C100" t="n">
         <v>0.1</v>
       </c>
@@ -11466,43 +11462,43 @@
         <v>70</v>
       </c>
       <c r="E100" t="s">
+        <v>314</v>
+      </c>
+      <c r="F100" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G100" t="n">
+        <v>70</v>
+      </c>
+      <c r="H100" t="s">
+        <v>314</v>
+      </c>
+      <c r="I100" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J100" t="n">
+        <v>70</v>
+      </c>
+      <c r="K100" t="s">
+        <v>314</v>
+      </c>
+      <c r="L100" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="M100" t="n">
+        <v>75</v>
+      </c>
+      <c r="N100" t="s">
         <v>315</v>
       </c>
-      <c r="F100" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="G100" t="n">
-        <v>70</v>
-      </c>
-      <c r="H100" t="s">
+      <c r="O100" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="P100" t="n">
+        <v>75</v>
+      </c>
+      <c r="Q100" t="s">
         <v>315</v>
-      </c>
-      <c r="I100" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="J100" t="n">
-        <v>70</v>
-      </c>
-      <c r="K100" t="s">
-        <v>315</v>
-      </c>
-      <c r="L100" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="M100" t="n">
-        <v>75</v>
-      </c>
-      <c r="N100" t="s">
-        <v>316</v>
-      </c>
-      <c r="O100" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="P100" t="n">
-        <v>75</v>
-      </c>
-      <c r="Q100" t="s">
-        <v>316</v>
       </c>
       <c r="R100" t="n">
         <v>0.2</v>
@@ -11552,10 +11548,10 @@
     </row>
     <row r="101">
       <c r="A101" t="s">
+        <v>321</v>
+      </c>
+      <c r="B101" t="s">
         <v>322</v>
-      </c>
-      <c r="B101" t="s">
-        <v>323</v>
       </c>
       <c r="C101" t="n">
         <v>0.1</v>
@@ -11650,11 +11646,11 @@
     </row>
     <row r="102">
       <c r="A102" t="s">
+        <v>323</v>
+      </c>
+      <c r="B102" t="s">
         <v>324</v>
       </c>
-      <c r="B102" t="s">
-        <v>325</v>
-      </c>
       <c r="C102" t="n">
         <v>0.1</v>
       </c>
@@ -11662,7 +11658,7 @@
         <v>70</v>
       </c>
       <c r="E102" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F102" t="n">
         <v>0.1</v>
@@ -11671,7 +11667,7 @@
         <v>70</v>
       </c>
       <c r="H102" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I102" t="n">
         <v>0.1</v>
@@ -11680,7 +11676,7 @@
         <v>70</v>
       </c>
       <c r="K102" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L102" t="n">
         <v>0.1</v>
@@ -11689,7 +11685,7 @@
         <v>70</v>
       </c>
       <c r="N102" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O102" t="n">
         <v>0.1</v>
@@ -11698,7 +11694,7 @@
         <v>70</v>
       </c>
       <c r="Q102" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="R102" t="n">
         <v>0.1</v>
@@ -11725,7 +11721,7 @@
         <v>70</v>
       </c>
       <c r="Z102" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AA102" t="n">
         <v>0.1</v>
@@ -11734,7 +11730,7 @@
         <v>70</v>
       </c>
       <c r="AC102" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AD102" t="n">
         <v>0.1</v>
@@ -11743,16 +11739,16 @@
         <v>70</v>
       </c>
       <c r="AF102" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
+        <v>325</v>
+      </c>
+      <c r="B103" t="s">
         <v>326</v>
       </c>
-      <c r="B103" t="s">
-        <v>327</v>
-      </c>
       <c r="C103" t="n">
         <v>0.1</v>
       </c>
@@ -11760,7 +11756,7 @@
         <v>70</v>
       </c>
       <c r="E103" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F103" t="n">
         <v>0.1</v>
@@ -11769,7 +11765,7 @@
         <v>70</v>
       </c>
       <c r="H103" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I103" t="n">
         <v>0.1</v>
@@ -11778,7 +11774,7 @@
         <v>70</v>
       </c>
       <c r="K103" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L103" t="n">
         <v>0.1</v>
@@ -11805,7 +11801,7 @@
         <v>85</v>
       </c>
       <c r="T103" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="U103" t="n">
         <v>0.1</v>
@@ -11814,7 +11810,7 @@
         <v>85</v>
       </c>
       <c r="W103" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="X103" t="n">
         <v>0.1</v>
@@ -11823,7 +11819,7 @@
         <v>70</v>
       </c>
       <c r="Z103" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AA103" t="n">
         <v>0.1</v>
@@ -11832,7 +11828,7 @@
         <v>70</v>
       </c>
       <c r="AC103" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AD103" t="n">
         <v>0.1</v>
@@ -11841,12 +11837,12 @@
         <v>70</v>
       </c>
       <c r="AF103" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B104"/>
       <c r="C104" t="n">
@@ -11883,7 +11879,7 @@
         <v>75</v>
       </c>
       <c r="N104" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="O104" t="n">
         <v>0.1</v>
@@ -11892,7 +11888,7 @@
         <v>75</v>
       </c>
       <c r="Q104" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="R104" t="n">
         <v>0.1</v>
@@ -11942,11 +11938,11 @@
     </row>
     <row r="105">
       <c r="A105" t="s">
+        <v>329</v>
+      </c>
+      <c r="B105" t="s">
         <v>330</v>
       </c>
-      <c r="B105" t="s">
-        <v>331</v>
-      </c>
       <c r="C105" t="n">
         <v>0.1</v>
       </c>
@@ -11954,7 +11950,7 @@
         <v>75</v>
       </c>
       <c r="E105" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F105" t="n">
         <v>0.1</v>
@@ -11963,7 +11959,7 @@
         <v>75</v>
       </c>
       <c r="H105" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I105" t="n">
         <v>0.1</v>
@@ -11972,7 +11968,7 @@
         <v>75</v>
       </c>
       <c r="K105" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L105" t="n">
         <v>0.1</v>
@@ -11981,7 +11977,7 @@
         <v>70</v>
       </c>
       <c r="N105" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O105" t="n">
         <v>0.1</v>
@@ -11990,7 +11986,7 @@
         <v>70</v>
       </c>
       <c r="Q105" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="R105" t="n">
         <v>0.1</v>
@@ -11999,7 +11995,7 @@
         <v>70</v>
       </c>
       <c r="T105" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="U105" t="n">
         <v>0.1</v>
@@ -12008,7 +12004,7 @@
         <v>70</v>
       </c>
       <c r="W105" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="X105" t="n">
         <v>0</v>
@@ -12017,7 +12013,7 @@
         <v>75</v>
       </c>
       <c r="Z105" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AA105" t="n">
         <v>0</v>
@@ -12026,7 +12022,7 @@
         <v>75</v>
       </c>
       <c r="AC105" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AD105" t="n">
         <v>0</v>
@@ -12035,15 +12031,15 @@
         <v>75</v>
       </c>
       <c r="AF105" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
+        <v>332</v>
+      </c>
+      <c r="B106" t="s">
         <v>333</v>
-      </c>
-      <c r="B106" t="s">
-        <v>334</v>
       </c>
       <c r="C106" t="n">
         <v>0.1</v>
@@ -12097,7 +12093,7 @@
         <v>75</v>
       </c>
       <c r="T106" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="U106" t="n">
         <v>0.1</v>
@@ -12106,7 +12102,7 @@
         <v>75</v>
       </c>
       <c r="W106" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="X106" t="n">
         <v>0.1</v>
@@ -12115,7 +12111,7 @@
         <v>75</v>
       </c>
       <c r="Z106" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AA106" t="n">
         <v>0.1</v>
@@ -12124,7 +12120,7 @@
         <v>75</v>
       </c>
       <c r="AC106" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AD106" t="n">
         <v>0.1</v>
@@ -12133,15 +12129,15 @@
         <v>75</v>
       </c>
       <c r="AF106" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
+        <v>334</v>
+      </c>
+      <c r="B107" t="s">
         <v>335</v>
-      </c>
-      <c r="B107" t="s">
-        <v>336</v>
       </c>
       <c r="C107" t="n">
         <v>-0.1</v>
@@ -12150,7 +12146,7 @@
         <v>70</v>
       </c>
       <c r="E107" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F107" t="n">
         <v>-0.1</v>
@@ -12159,7 +12155,7 @@
         <v>70</v>
       </c>
       <c r="H107" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I107" t="n">
         <v>-0.1</v>
@@ -12168,7 +12164,7 @@
         <v>70</v>
       </c>
       <c r="K107" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L107" t="n">
         <v>-0.1</v>
@@ -12177,7 +12173,7 @@
         <v>65</v>
       </c>
       <c r="N107" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O107" t="n">
         <v>-0.1</v>
@@ -12186,7 +12182,7 @@
         <v>65</v>
       </c>
       <c r="Q107" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="R107" t="n">
         <v>-0.1</v>
@@ -12195,7 +12191,7 @@
         <v>70</v>
       </c>
       <c r="T107" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U107" t="n">
         <v>-0.1</v>
@@ -12204,7 +12200,7 @@
         <v>70</v>
       </c>
       <c r="W107" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="X107" t="n">
         <v>-0.1</v>
@@ -12213,7 +12209,7 @@
         <v>70</v>
       </c>
       <c r="Z107" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AA107" t="n">
         <v>-0.1</v>
@@ -12222,7 +12218,7 @@
         <v>70</v>
       </c>
       <c r="AC107" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AD107" t="n">
         <v>-0.1</v>
@@ -12231,12 +12227,12 @@
         <v>70</v>
       </c>
       <c r="AF107" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B108"/>
       <c r="C108" t="n">
@@ -12273,7 +12269,7 @@
         <v>70</v>
       </c>
       <c r="N108" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="O108" t="n">
         <v>-0.1</v>
@@ -12282,7 +12278,7 @@
         <v>70</v>
       </c>
       <c r="Q108" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="R108" t="n">
         <v>0</v>
@@ -12291,7 +12287,7 @@
         <v>70</v>
       </c>
       <c r="T108" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="U108" t="n">
         <v>0</v>
@@ -12300,7 +12296,7 @@
         <v>70</v>
       </c>
       <c r="W108" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="X108" t="n">
         <v>0</v>
@@ -12332,10 +12328,10 @@
     </row>
     <row r="109">
       <c r="A109" t="s">
+        <v>338</v>
+      </c>
+      <c r="B109" t="s">
         <v>339</v>
-      </c>
-      <c r="B109" t="s">
-        <v>340</v>
       </c>
       <c r="C109" t="n">
         <v>-0.1</v>
@@ -12344,7 +12340,7 @@
         <v>70</v>
       </c>
       <c r="E109" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F109" t="n">
         <v>-0.1</v>
@@ -12353,7 +12349,7 @@
         <v>70</v>
       </c>
       <c r="H109" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I109" t="n">
         <v>-0.1</v>
@@ -12362,7 +12358,7 @@
         <v>70</v>
       </c>
       <c r="K109" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L109" t="n">
         <v>0</v>
@@ -12430,7 +12426,7 @@
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B110"/>
       <c r="C110" t="n">
@@ -12526,11 +12522,11 @@
     </row>
     <row r="111">
       <c r="A111" t="s">
+        <v>341</v>
+      </c>
+      <c r="B111" t="s">
         <v>342</v>
       </c>
-      <c r="B111" t="s">
-        <v>343</v>
-      </c>
       <c r="C111" t="n">
         <v>0.1</v>
       </c>
@@ -12538,7 +12534,7 @@
         <v>70</v>
       </c>
       <c r="E111" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F111" t="n">
         <v>0.1</v>
@@ -12547,7 +12543,7 @@
         <v>70</v>
       </c>
       <c r="H111" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I111" t="n">
         <v>0.1</v>
@@ -12556,7 +12552,7 @@
         <v>70</v>
       </c>
       <c r="K111" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L111" t="n">
         <v>0.1</v>
@@ -12624,10 +12620,10 @@
     </row>
     <row r="112">
       <c r="A112" t="s">
+        <v>343</v>
+      </c>
+      <c r="B112" t="s">
         <v>344</v>
-      </c>
-      <c r="B112" t="s">
-        <v>345</v>
       </c>
       <c r="C112" t="n">
         <v>0.2</v>
@@ -12722,10 +12718,10 @@
     </row>
     <row r="113">
       <c r="A113" t="s">
+        <v>345</v>
+      </c>
+      <c r="B113" t="s">
         <v>346</v>
-      </c>
-      <c r="B113" t="s">
-        <v>347</v>
       </c>
       <c r="C113" t="n">
         <v>0.1</v>
@@ -12779,7 +12775,7 @@
         <v>70</v>
       </c>
       <c r="T113" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="U113" t="n">
         <v>0.1</v>
@@ -12788,7 +12784,7 @@
         <v>70</v>
       </c>
       <c r="W113" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="X113" t="n">
         <v>0.1</v>
@@ -12820,10 +12816,10 @@
     </row>
     <row r="114">
       <c r="A114" t="s">
+        <v>347</v>
+      </c>
+      <c r="B114" t="s">
         <v>348</v>
-      </c>
-      <c r="B114" t="s">
-        <v>349</v>
       </c>
       <c r="C114" t="n">
         <v>0.1</v>
@@ -12877,7 +12873,7 @@
         <v>70</v>
       </c>
       <c r="T114" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="U114" t="n">
         <v>0.1</v>
@@ -12886,7 +12882,7 @@
         <v>70</v>
       </c>
       <c r="W114" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="X114" t="n">
         <v>0.1</v>
@@ -12918,10 +12914,10 @@
     </row>
     <row r="115">
       <c r="A115" t="s">
+        <v>349</v>
+      </c>
+      <c r="B115" t="s">
         <v>350</v>
-      </c>
-      <c r="B115" t="s">
-        <v>351</v>
       </c>
       <c r="C115" t="n">
         <v>0.1</v>
@@ -12975,7 +12971,7 @@
         <v>75</v>
       </c>
       <c r="T115" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="U115" t="n">
         <v>0</v>
@@ -12984,7 +12980,7 @@
         <v>75</v>
       </c>
       <c r="W115" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="X115" t="n">
         <v>0.1</v>
@@ -12993,7 +12989,7 @@
         <v>75</v>
       </c>
       <c r="Z115" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AA115" t="n">
         <v>0.1</v>
@@ -13002,7 +12998,7 @@
         <v>75</v>
       </c>
       <c r="AC115" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AD115" t="n">
         <v>0.1</v>
@@ -13011,12 +13007,12 @@
         <v>75</v>
       </c>
       <c r="AF115" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B116"/>
       <c r="C116" t="n">
@@ -13026,7 +13022,7 @@
         <v>65</v>
       </c>
       <c r="E116" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F116" t="n">
         <v>-0.2</v>
@@ -13035,7 +13031,7 @@
         <v>65</v>
       </c>
       <c r="H116" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="I116" t="n">
         <v>-0.2</v>
@@ -13044,7 +13040,7 @@
         <v>65</v>
       </c>
       <c r="K116" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="L116" t="n">
         <v>-0.1</v>
@@ -13053,7 +13049,7 @@
         <v>65</v>
       </c>
       <c r="N116" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O116" t="n">
         <v>-0.1</v>
@@ -13062,7 +13058,7 @@
         <v>65</v>
       </c>
       <c r="Q116" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="R116" t="n">
         <v>-0.1</v>
@@ -13089,7 +13085,7 @@
         <v>65</v>
       </c>
       <c r="Z116" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="AA116" t="n">
         <v>-0.2</v>
@@ -13098,7 +13094,7 @@
         <v>65</v>
       </c>
       <c r="AC116" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="AD116" t="n">
         <v>-0.2</v>
@@ -13107,15 +13103,15 @@
         <v>65</v>
       </c>
       <c r="AF116" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="s">
+        <v>353</v>
+      </c>
+      <c r="B117" t="s">
         <v>354</v>
-      </c>
-      <c r="B117" t="s">
-        <v>355</v>
       </c>
       <c r="C117" t="n">
         <v>0.2</v>
@@ -13210,10 +13206,10 @@
     </row>
     <row r="118">
       <c r="A118" t="s">
+        <v>355</v>
+      </c>
+      <c r="B118" t="s">
         <v>356</v>
-      </c>
-      <c r="B118" t="s">
-        <v>357</v>
       </c>
       <c r="C118" t="n">
         <v>-0.1</v>
@@ -13222,7 +13218,7 @@
         <v>70</v>
       </c>
       <c r="E118" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F118" t="n">
         <v>-0.1</v>
@@ -13231,7 +13227,7 @@
         <v>70</v>
       </c>
       <c r="H118" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I118" t="n">
         <v>-0.1</v>
@@ -13240,7 +13236,7 @@
         <v>70</v>
       </c>
       <c r="K118" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L118" t="n">
         <v>0.1</v>
@@ -13249,7 +13245,7 @@
         <v>70</v>
       </c>
       <c r="N118" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O118" t="n">
         <v>0.1</v>
@@ -13258,7 +13254,7 @@
         <v>70</v>
       </c>
       <c r="Q118" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="R118" t="n">
         <v>0</v>
@@ -13267,7 +13263,7 @@
         <v>75</v>
       </c>
       <c r="T118" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="U118" t="n">
         <v>0</v>
@@ -13276,7 +13272,7 @@
         <v>75</v>
       </c>
       <c r="W118" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="X118" t="n">
         <v>0</v>
@@ -13285,7 +13281,7 @@
         <v>75</v>
       </c>
       <c r="Z118" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AA118" t="n">
         <v>0</v>
@@ -13294,7 +13290,7 @@
         <v>75</v>
       </c>
       <c r="AC118" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AD118" t="n">
         <v>0</v>
@@ -13303,15 +13299,15 @@
         <v>75</v>
       </c>
       <c r="AF118" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="s">
+        <v>357</v>
+      </c>
+      <c r="B119" t="s">
         <v>358</v>
-      </c>
-      <c r="B119" t="s">
-        <v>359</v>
       </c>
       <c r="C119" t="n">
         <v>0.1</v>
@@ -13320,7 +13316,7 @@
         <v>55</v>
       </c>
       <c r="E119" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F119" t="n">
         <v>-0.1</v>
@@ -13329,7 +13325,7 @@
         <v>45</v>
       </c>
       <c r="H119" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="I119" t="n">
         <v>-0.1</v>
@@ -13338,7 +13334,7 @@
         <v>45</v>
       </c>
       <c r="K119" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="L119" t="n">
         <v>-0.1</v>
@@ -13347,7 +13343,7 @@
         <v>60</v>
       </c>
       <c r="N119" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="O119" t="n">
         <v>-0.1</v>
@@ -13356,7 +13352,7 @@
         <v>60</v>
       </c>
       <c r="Q119" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R119" t="n">
         <v>-0.1</v>
@@ -13365,7 +13361,7 @@
         <v>65</v>
       </c>
       <c r="T119" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="U119" t="n">
         <v>-0.1</v>
@@ -13374,7 +13370,7 @@
         <v>65</v>
       </c>
       <c r="W119" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="X119" t="n">
         <v>-0.1</v>
@@ -13383,7 +13379,7 @@
         <v>55</v>
       </c>
       <c r="Z119" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AA119" t="n">
         <v>-0.1</v>
@@ -13392,7 +13388,7 @@
         <v>55</v>
       </c>
       <c r="AC119" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AD119" t="n">
         <v>-0.1</v>
@@ -13401,12 +13397,12 @@
         <v>55</v>
       </c>
       <c r="AF119" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B120"/>
       <c r="C120" t="n">
@@ -13416,7 +13412,7 @@
         <v>80</v>
       </c>
       <c r="E120" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F120" t="n">
         <v>-0.1</v>
@@ -13425,7 +13421,7 @@
         <v>80</v>
       </c>
       <c r="H120" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I120" t="n">
         <v>-0.1</v>
@@ -13434,7 +13430,7 @@
         <v>80</v>
       </c>
       <c r="K120" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="L120" t="n">
         <v>0</v>
@@ -13443,7 +13439,7 @@
         <v>60</v>
       </c>
       <c r="N120" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="O120" t="n">
         <v>0</v>
@@ -13452,7 +13448,7 @@
         <v>60</v>
       </c>
       <c r="Q120" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="R120" t="n">
         <v>-0.1</v>
@@ -13502,10 +13498,10 @@
     </row>
     <row r="121">
       <c r="A121" t="s">
+        <v>362</v>
+      </c>
+      <c r="B121" t="s">
         <v>363</v>
-      </c>
-      <c r="B121" t="s">
-        <v>364</v>
       </c>
       <c r="C121" t="n">
         <v>-0.1</v>
@@ -13514,7 +13510,7 @@
         <v>80</v>
       </c>
       <c r="E121" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F121" t="n">
         <v>-0.1</v>
@@ -13523,7 +13519,7 @@
         <v>80</v>
       </c>
       <c r="H121" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I121" t="n">
         <v>-0.1</v>
@@ -13532,7 +13528,7 @@
         <v>80</v>
       </c>
       <c r="K121" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="L121" t="n">
         <v>-0.1</v>
@@ -13541,7 +13537,7 @@
         <v>85</v>
       </c>
       <c r="N121" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="O121" t="n">
         <v>-0.1</v>
@@ -13550,7 +13546,7 @@
         <v>85</v>
       </c>
       <c r="Q121" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="R121" t="n">
         <v>-0.1</v>
@@ -13559,7 +13555,7 @@
         <v>70</v>
       </c>
       <c r="T121" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U121" t="n">
         <v>-0.1</v>
@@ -13568,7 +13564,7 @@
         <v>70</v>
       </c>
       <c r="W121" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="X121" t="n">
         <v>-0.1</v>
@@ -13577,7 +13573,7 @@
         <v>70</v>
       </c>
       <c r="Z121" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AA121" t="n">
         <v>-0.1</v>
@@ -13586,7 +13582,7 @@
         <v>70</v>
       </c>
       <c r="AC121" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AD121" t="n">
         <v>-0.1</v>
@@ -13595,12 +13591,12 @@
         <v>70</v>
       </c>
       <c r="AF121" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B122"/>
       <c r="C122" t="n">
@@ -13696,10 +13692,10 @@
     </row>
     <row r="123">
       <c r="A123" t="s">
+        <v>366</v>
+      </c>
+      <c r="B123" t="s">
         <v>367</v>
-      </c>
-      <c r="B123" t="s">
-        <v>368</v>
       </c>
       <c r="C123" t="n">
         <v>0.1</v>
@@ -13708,7 +13704,7 @@
         <v>55</v>
       </c>
       <c r="E123" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F123" t="n">
         <v>0.1</v>
@@ -13717,7 +13713,7 @@
         <v>55</v>
       </c>
       <c r="H123" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I123" t="n">
         <v>0.1</v>
@@ -13726,7 +13722,7 @@
         <v>55</v>
       </c>
       <c r="K123" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L123" t="n">
         <v>0.1</v>
@@ -13794,10 +13790,10 @@
     </row>
     <row r="124">
       <c r="A124" t="s">
+        <v>368</v>
+      </c>
+      <c r="B124" t="s">
         <v>369</v>
-      </c>
-      <c r="B124" t="s">
-        <v>370</v>
       </c>
       <c r="C124" t="n">
         <v>-0.1</v>
@@ -13833,7 +13829,7 @@
         <v>85</v>
       </c>
       <c r="N124" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="O124" t="n">
         <v>-0.1</v>
@@ -13842,7 +13838,7 @@
         <v>85</v>
       </c>
       <c r="Q124" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="R124" t="n">
         <v>-0.1</v>
@@ -13851,7 +13847,7 @@
         <v>70</v>
       </c>
       <c r="T124" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="U124" t="n">
         <v>-0.1</v>
@@ -13860,7 +13856,7 @@
         <v>70</v>
       </c>
       <c r="W124" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="X124" t="n">
         <v>0</v>
@@ -13869,7 +13865,7 @@
         <v>75</v>
       </c>
       <c r="Z124" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AA124" t="n">
         <v>0</v>
@@ -13878,7 +13874,7 @@
         <v>75</v>
       </c>
       <c r="AC124" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AD124" t="n">
         <v>0</v>
@@ -13887,15 +13883,15 @@
         <v>75</v>
       </c>
       <c r="AF124" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="s">
+        <v>370</v>
+      </c>
+      <c r="B125" t="s">
         <v>371</v>
-      </c>
-      <c r="B125" t="s">
-        <v>372</v>
       </c>
       <c r="C125" t="n">
         <v>0.1</v>
@@ -13990,10 +13986,10 @@
     </row>
     <row r="126">
       <c r="A126" t="s">
+        <v>372</v>
+      </c>
+      <c r="B126" t="s">
         <v>373</v>
-      </c>
-      <c r="B126" t="s">
-        <v>374</v>
       </c>
       <c r="C126" t="n">
         <v>-0.1</v>
@@ -14002,7 +13998,7 @@
         <v>70</v>
       </c>
       <c r="E126" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F126" t="n">
         <v>-0.1</v>
@@ -14011,7 +14007,7 @@
         <v>70</v>
       </c>
       <c r="H126" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I126" t="n">
         <v>-0.1</v>
@@ -14020,7 +14016,7 @@
         <v>70</v>
       </c>
       <c r="K126" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L126" t="n">
         <v>-0.1</v>
@@ -14029,7 +14025,7 @@
         <v>70</v>
       </c>
       <c r="N126" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="O126" t="n">
         <v>-0.1</v>
@@ -14038,7 +14034,7 @@
         <v>70</v>
       </c>
       <c r="Q126" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="R126" t="n">
         <v>-0.1</v>
@@ -14047,7 +14043,7 @@
         <v>65</v>
       </c>
       <c r="T126" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="U126" t="n">
         <v>-0.1</v>
@@ -14056,7 +14052,7 @@
         <v>65</v>
       </c>
       <c r="W126" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="X126" t="n">
         <v>-0.1</v>
@@ -14065,7 +14061,7 @@
         <v>70</v>
       </c>
       <c r="Z126" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AA126" t="n">
         <v>-0.1</v>
@@ -14074,7 +14070,7 @@
         <v>70</v>
       </c>
       <c r="AC126" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AD126" t="n">
         <v>-0.1</v>
@@ -14083,15 +14079,15 @@
         <v>70</v>
       </c>
       <c r="AF126" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="s">
+        <v>374</v>
+      </c>
+      <c r="B127" t="s">
         <v>375</v>
-      </c>
-      <c r="B127" t="s">
-        <v>376</v>
       </c>
       <c r="C127" t="n">
         <v>-0.1</v>
@@ -14145,7 +14141,7 @@
         <v>75</v>
       </c>
       <c r="T127" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="U127" t="n">
         <v>0</v>
@@ -14154,7 +14150,7 @@
         <v>75</v>
       </c>
       <c r="W127" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="X127" t="n">
         <v>-0.1</v>
@@ -14186,7 +14182,7 @@
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B128"/>
       <c r="C128" t="n">
@@ -14196,7 +14192,7 @@
         <v>65</v>
       </c>
       <c r="E128" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F128" t="n">
         <v>-0.1</v>
@@ -14205,7 +14201,7 @@
         <v>65</v>
       </c>
       <c r="H128" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I128" t="n">
         <v>-0.1</v>
@@ -14214,7 +14210,7 @@
         <v>65</v>
       </c>
       <c r="K128" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="L128" t="n">
         <v>0.1</v>
@@ -14259,7 +14255,7 @@
         <v>55</v>
       </c>
       <c r="Z128" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AA128" t="n">
         <v>-0.1</v>
@@ -14268,7 +14264,7 @@
         <v>55</v>
       </c>
       <c r="AC128" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AD128" t="n">
         <v>-0.1</v>
@@ -14277,15 +14273,15 @@
         <v>55</v>
       </c>
       <c r="AF128" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="s">
+        <v>377</v>
+      </c>
+      <c r="B129" t="s">
         <v>378</v>
-      </c>
-      <c r="B129" t="s">
-        <v>379</v>
       </c>
       <c r="C129" t="n">
         <v>-0.1</v>
@@ -14294,7 +14290,7 @@
         <v>65</v>
       </c>
       <c r="E129" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F129" t="n">
         <v>-0.1</v>
@@ -14303,7 +14299,7 @@
         <v>65</v>
       </c>
       <c r="H129" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I129" t="n">
         <v>-0.1</v>
@@ -14312,7 +14308,7 @@
         <v>65</v>
       </c>
       <c r="K129" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="L129" t="n">
         <v>-0.1</v>
@@ -14321,7 +14317,7 @@
         <v>65</v>
       </c>
       <c r="N129" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O129" t="n">
         <v>-0.1</v>
@@ -14330,7 +14326,7 @@
         <v>65</v>
       </c>
       <c r="Q129" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="R129" t="n">
         <v>-0.1</v>
@@ -14380,10 +14376,10 @@
     </row>
     <row r="130">
       <c r="A130" t="s">
+        <v>379</v>
+      </c>
+      <c r="B130" t="s">
         <v>380</v>
-      </c>
-      <c r="B130" t="s">
-        <v>381</v>
       </c>
       <c r="C130" t="n">
         <v>0.2</v>
@@ -14437,7 +14433,7 @@
         <v>70</v>
       </c>
       <c r="T130" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="U130" t="n">
         <v>0.1</v>
@@ -14446,7 +14442,7 @@
         <v>70</v>
       </c>
       <c r="W130" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="X130" t="n">
         <v>0.1</v>
@@ -14478,10 +14474,10 @@
     </row>
     <row r="131">
       <c r="A131" t="s">
+        <v>381</v>
+      </c>
+      <c r="B131" t="s">
         <v>382</v>
-      </c>
-      <c r="B131" t="s">
-        <v>383</v>
       </c>
       <c r="C131" t="n">
         <v>0.1</v>
@@ -14517,7 +14513,7 @@
         <v>65</v>
       </c>
       <c r="N131" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O131" t="n">
         <v>0.1</v>
@@ -14526,7 +14522,7 @@
         <v>70</v>
       </c>
       <c r="Q131" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="R131" t="n">
         <v>0.1</v>
@@ -14553,7 +14549,7 @@
         <v>45</v>
       </c>
       <c r="Z131" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="AA131" t="n">
         <v>-0.1</v>
@@ -14562,7 +14558,7 @@
         <v>45</v>
       </c>
       <c r="AC131" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="AD131" t="n">
         <v>-0.1</v>
@@ -14571,7 +14567,7 @@
         <v>45</v>
       </c>
       <c r="AF131" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>

</xml_diff>